<commit_message>
Final 2020 changes to files
</commit_message>
<xml_diff>
--- a/Bill_of_Materials.xlsx
+++ b/Bill_of_Materials.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802C0F99-5644-4DA3-A828-96DC4EDB2FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{802C0F99-5644-4DA3-A828-96DC4EDB2FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A3D521B-129A-4530-B0F7-5BF6E8D67E88}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resonant Converter" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="189">
   <si>
     <t>***  Sheet to remain hidden ***</t>
   </si>
@@ -129,9 +129,6 @@
     <t>BB Inductor</t>
   </si>
   <si>
-    <t>PMEG2010AEH</t>
-  </si>
-  <si>
     <t>10 uF</t>
   </si>
   <si>
@@ -216,18 +213,12 @@
     <t>Output Capacitor</t>
   </si>
   <si>
-    <t>27 k</t>
-  </si>
-  <si>
     <t>113 k</t>
   </si>
   <si>
     <t>18 k</t>
   </si>
   <si>
-    <t>3.3 uH</t>
-  </si>
-  <si>
     <t>25 m</t>
   </si>
   <si>
@@ -267,9 +258,6 @@
     <t>12 uH</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Taiyo-Yuden/LBM2016T3R3J?qs=PzICbMaShUf8XTCkSPcMgA%3D%3D</t>
-  </si>
-  <si>
     <t>47 nF</t>
   </si>
   <si>
@@ -279,12 +267,6 @@
     <t>https://www.mouser.com/ProductDetail/Yageo/CC0603KRX7R9BB104?qs=sGAEpiMZZMvsSlwiRhF8qgFnKIgZe697WZ9nrpNTeGg%3D</t>
   </si>
   <si>
-    <t>1.5 nF</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Panasonic/ECH-U1C152GX5?qs=b%252BB9euYP3EOFYa2PCy7ENw%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/KEMET/C0603C103J5RACTU?qs=sGAEpiMZZMvsSlwiRhF8quIsB1QHp5lf6wge94WzHBg%3D</t>
   </si>
   <si>
@@ -294,9 +276,6 @@
     <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF3R00?qs=sGAEpiMZZMvdGkrng054t621aZ%2Fa1rARaVFHqRTCm0PPnIKjieahpQ%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Panasonic/ERA-3AED273V?qs=sGAEpiMZZMvdGkrng054t5mej2KPdPuF%2FumH4pW8%2FtA%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Bourns/CR0805-FX-1133ELF?qs=sGAEpiMZZMvdGkrng054t%252BRNGJdg958RyANX4l%252BOsPU%3D</t>
   </si>
   <si>
@@ -312,9 +291,6 @@
     <t>https://www.mouser.com/ProductDetail/Yageo/RC0603FR-0747KL?qs=sGAEpiMZZMvdGkrng054t8Tx25L%252BvTaR3%2FWJtGCqf3I%3D</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/750342864?qs=%2Fha2pyFaduiPL7J5PpgfMP4%252BxDENdIFQUex44KftFGZy5Bz7I%252BzpTA%3D%3D</t>
   </si>
   <si>
@@ -333,21 +309,12 @@
     <t>Magnetizing Inductor</t>
   </si>
   <si>
-    <t>LBM2016T3R3J</t>
-  </si>
-  <si>
     <t>CR0805-FX-1133ELF</t>
   </si>
   <si>
     <t>CRCW080518K0FKEA</t>
   </si>
   <si>
-    <t>ERA-3AED273V</t>
-  </si>
-  <si>
-    <t>ECH-U1C152GX5</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB104</t>
   </si>
   <si>
@@ -589,6 +556,51 @@
   </si>
   <si>
     <t>AC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>24 k</t>
+  </si>
+  <si>
+    <t>3.3 nF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ERA-3AED243V?qs=SWVmE3OSrOmwxrbbukvP0g%3D%3D</t>
+  </si>
+  <si>
+    <t>ERA-3AED243V</t>
+  </si>
+  <si>
+    <t>ECH-U1C332GX5</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ECH-U1C332GX5?qs=O9nxk9bDVAjmIw2e8gOaeQ%3D%3D</t>
+  </si>
+  <si>
+    <t>6.8 uH</t>
+  </si>
+  <si>
+    <t>CB2016T6R8M</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Taiyo-Yuden/CB2016T6R8M?qs=I6KAKw0tg2zlZTrvjf8dKA%3D%3D</t>
+  </si>
+  <si>
+    <t>J5+</t>
+  </si>
+  <si>
+    <t>J1...J4</t>
+  </si>
+  <si>
+    <t>PMEG2010AEH,115</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/87891-0106?qs=kNSQ05%252BLZoC2%252Bs81B6ycXA%3D%3D</t>
+  </si>
+  <si>
+    <t>Single Headers</t>
+  </si>
+  <si>
+    <t>87891-0106</t>
   </si>
 </sst>
 </file>
@@ -953,203 +965,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="White Background" xfId="5" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill>
@@ -1253,6 +1069,209 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="8"/>
       </font>
@@ -1272,9 +1291,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Grocery List" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="40"/>
-      <tableStyleElement type="headerRow" dxfId="39"/>
-      <tableStyleElement type="firstRowStripe" dxfId="38"/>
+      <tableStyleElement type="wholeTable" dxfId="41"/>
+      <tableStyleElement type="headerRow" dxfId="40"/>
+      <tableStyleElement type="firstRowStripe" dxfId="39"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1289,20 +1308,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6EF63065-419A-4D8F-A7C2-A5B4F794B74F}" name="List3" displayName="List3" ref="C3:M47" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="White Background">
-  <autoFilter ref="C3:M47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6EF63065-419A-4D8F-A7C2-A5B4F794B74F}" name="List3" displayName="List3" ref="C3:M48" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="White Background">
+  <autoFilter ref="C3:M48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{4A4F8B4D-A5B3-42DD-A706-7F4F15C9EA13}" name="Bought" dataDxfId="37" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{001647D6-B767-481B-946E-C6F530EF1A94}" name="Item Name" dataDxfId="36" dataCellStyle="Item"/>
-    <tableColumn id="9" xr3:uid="{71CAAABD-DFED-4BD6-B894-1BE430159FE1}" name="Component Label" dataDxfId="35" dataCellStyle="White Background"/>
-    <tableColumn id="3" xr3:uid="{7B3DAD00-1931-4B1F-A607-6C8342CC212D}" name="Part Number" dataDxfId="34" dataCellStyle="White Background"/>
-    <tableColumn id="10" xr3:uid="{22EA3EC1-E4F4-4068-85D6-898D1C5D34D4}" name="Value" dataDxfId="33" dataCellStyle="White Background"/>
-    <tableColumn id="4" xr3:uid="{E54B3D03-9BB5-49D1-B4EC-D7992901BE9C}" name="QTY" dataDxfId="32" dataCellStyle="White Background"/>
-    <tableColumn id="5" xr3:uid="{A539EC19-D604-4FD5-AC9A-DC14BCF73F44}" name="Price" dataDxfId="31" dataCellStyle="Currency Custom"/>
-    <tableColumn id="6" xr3:uid="{EC7EC7B4-3813-47E4-BB03-F0807F9F27E3}" name="Total" dataDxfId="30" dataCellStyle="Currency Custom">
+    <tableColumn id="1" xr3:uid="{4A4F8B4D-A5B3-42DD-A706-7F4F15C9EA13}" name="Bought" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{001647D6-B767-481B-946E-C6F530EF1A94}" name="Item Name" dataDxfId="8" dataCellStyle="Item"/>
+    <tableColumn id="9" xr3:uid="{71CAAABD-DFED-4BD6-B894-1BE430159FE1}" name="Component Label" dataDxfId="7" dataCellStyle="White Background"/>
+    <tableColumn id="3" xr3:uid="{7B3DAD00-1931-4B1F-A607-6C8342CC212D}" name="Part Number" dataDxfId="6" dataCellStyle="White Background"/>
+    <tableColumn id="10" xr3:uid="{22EA3EC1-E4F4-4068-85D6-898D1C5D34D4}" name="Value" dataDxfId="5" dataCellStyle="White Background"/>
+    <tableColumn id="4" xr3:uid="{E54B3D03-9BB5-49D1-B4EC-D7992901BE9C}" name="QTY" dataDxfId="4" dataCellStyle="White Background"/>
+    <tableColumn id="5" xr3:uid="{A539EC19-D604-4FD5-AC9A-DC14BCF73F44}" name="Price" dataDxfId="3" dataCellStyle="Currency Custom"/>
+    <tableColumn id="6" xr3:uid="{EC7EC7B4-3813-47E4-BB03-F0807F9F27E3}" name="Total" dataDxfId="2" dataCellStyle="Currency Custom">
       <calculatedColumnFormula>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0D6E47E1-E149-4041-8FD9-1950CF4DF3D8}" name="Datasheet URL" dataDxfId="29" dataCellStyle="Indent"/>
+    <tableColumn id="7" xr3:uid="{0D6E47E1-E149-4041-8FD9-1950CF4DF3D8}" name="Datasheet URL" dataDxfId="1" dataCellStyle="Indent"/>
     <tableColumn id="8" xr3:uid="{60E7C40D-4AEC-4010-B833-DA3EAAF8AA2B}" name="Column1" dataCellStyle="White Background"/>
     <tableColumn id="11" xr3:uid="{A8E1CEB1-8209-4DDD-B608-A5F75345FEC0}" name="Column2" dataCellStyle="White Background"/>
   </tableColumns>
@@ -1546,10 +1565,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1560,11 +1579,11 @@
     <col min="4" max="4" width="23.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="100" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="103.44140625" style="3" customWidth="1"/>
     <col min="12" max="12" width="33.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="10"/>
@@ -1631,22 +1650,22 @@
         <v>20</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C4" s="9"/>
       <c r="D4" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>13</v>
@@ -1662,7 +1681,7 @@
         <v>36</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="26"/>
@@ -1670,13 +1689,13 @@
     <row r="5" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="9"/>
       <c r="D5" s="16" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>13</v>
@@ -1692,7 +1711,7 @@
         <v>20.52</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="26"/>
@@ -1700,59 +1719,59 @@
     <row r="6" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>17</v>
+        <v>187</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>188</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="17">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I6" s="18">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="J6" s="18">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>2.2200000000000002</v>
+        <v>0.21</v>
+      </c>
+      <c r="J6" s="19">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>2.94</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="L6" s="21"/>
-      <c r="M6" s="27"/>
+      <c r="M6" s="26"/>
     </row>
     <row r="7" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C7" s="9"/>
       <c r="D7" s="16" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>139</v>
+        <v>51</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="G7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" s="18">
-        <v>0.92</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J7" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>3.68</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="27"/>
@@ -1763,10 +1782,10 @@
         <v>56</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>153</v>
+        <v>100</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>128</v>
       </c>
       <c r="G8" s="34" t="s">
         <v>13</v>
@@ -1775,74 +1794,74 @@
         <v>4</v>
       </c>
       <c r="I8" s="18">
-        <v>0.57999999999999996</v>
+        <v>1.06</v>
       </c>
       <c r="J8" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>2.3199999999999998</v>
+        <v>4.24</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L8" s="21"/>
-      <c r="M8" s="28"/>
+      <c r="M8" s="27"/>
     </row>
     <row r="9" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="9"/>
       <c r="D9" s="16" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="20">
-        <v>750342864</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>65</v>
+        <v>101</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="H9" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" s="18">
-        <v>5.76</v>
+        <v>0.8</v>
       </c>
       <c r="J9" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>5.76</v>
+        <v>3.2</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="L9" s="21"/>
-      <c r="M9" s="26"/>
+      <c r="M9" s="28"/>
     </row>
     <row r="10" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="9"/>
       <c r="D10" s="16" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="35">
-        <v>744373965120</v>
+        <v>102</v>
+      </c>
+      <c r="F10" s="20">
+        <v>750342864</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="H10" s="17">
         <v>1</v>
       </c>
       <c r="I10" s="18">
-        <v>2.81</v>
-      </c>
-      <c r="J10" s="19">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>2.81</v>
+        <v>5.76</v>
+      </c>
+      <c r="J10" s="18">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>5.76</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="26"/>
@@ -1850,29 +1869,29 @@
     <row r="11" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="9"/>
       <c r="D11" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="F11" s="35">
+        <v>744373965120</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H11" s="17">
         <v>1</v>
       </c>
       <c r="I11" s="18">
-        <v>1.71</v>
+        <v>2.81</v>
       </c>
       <c r="J11" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>1.71</v>
+        <v>2.81</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="L11" s="21"/>
       <c r="M11" s="26"/>
@@ -1880,29 +1899,29 @@
     <row r="12" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="9"/>
       <c r="D12" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="H12" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="18">
-        <v>0.71</v>
+        <v>1.71</v>
       </c>
       <c r="J12" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>1.42</v>
+        <v>1.71</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="26"/>
@@ -1910,76 +1929,76 @@
     <row r="13" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="9"/>
       <c r="D13" s="16" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="35">
-        <v>744373965120</v>
+        <v>127</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="H13" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" s="18">
-        <v>2.81</v>
+        <v>0.71</v>
       </c>
       <c r="J13" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>8.43</v>
+        <v>1.42</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="L13" s="21"/>
       <c r="M13" s="26"/>
     </row>
-    <row r="14" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="9"/>
       <c r="D14" s="16" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>151</v>
+        <v>104</v>
+      </c>
+      <c r="F14" s="35">
+        <v>744373965120</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="H14" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" s="18">
-        <v>0.3</v>
+        <v>2.81</v>
       </c>
       <c r="J14" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.6</v>
+        <v>8.43</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
+      <c r="M14" s="26"/>
     </row>
     <row r="15" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="9"/>
       <c r="D15" s="16" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>151</v>
+        <v>105</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>140</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="17">
         <v>2</v>
@@ -1992,7 +2011,7 @@
         <v>0.6</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
@@ -2000,29 +2019,29 @@
     <row r="16" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="9"/>
       <c r="D16" s="16" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>141</v>
+        <v>49</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H16" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="18">
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="J16" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.48</v>
+        <v>0.6</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
@@ -2030,29 +2049,29 @@
     <row r="17" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C17" s="9"/>
       <c r="D17" s="16" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>151</v>
+        <v>107</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>130</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H17" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="18">
-        <v>0.3</v>
+        <v>0.48</v>
       </c>
       <c r="J17" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.6</v>
+        <v>0.48</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
@@ -2060,29 +2079,29 @@
     <row r="18" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="9"/>
       <c r="D18" s="16" t="s">
-        <v>162</v>
+        <v>58</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>184</v>
+        <v>50</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="H18" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="18">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J18" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
@@ -2090,16 +2109,16 @@
     <row r="19" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="9"/>
       <c r="D19" s="16" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>181</v>
+        <v>153</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>173</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H19" s="17">
         <v>1</v>
@@ -2112,7 +2131,7 @@
         <v>0.1</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -2120,29 +2139,29 @@
     <row r="20" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C20" s="9"/>
       <c r="D20" s="16" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>180</v>
+        <v>154</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>170</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="18">
         <v>0.1</v>
       </c>
       <c r="J20" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2150,73 +2169,73 @@
     <row r="21" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C21" s="9"/>
       <c r="D21" s="16" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>155</v>
+        <v>160</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>169</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="H21" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" s="18">
-        <v>0.84</v>
+        <v>0.1</v>
       </c>
       <c r="J21" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.84</v>
+        <v>0.2</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
     </row>
-    <row r="22" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C22" s="9"/>
       <c r="D22" s="16" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="34" t="s">
-        <v>13</v>
+        <v>108</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="H22" s="17">
         <v>1</v>
       </c>
       <c r="I22" s="18">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="J22" s="18">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>2.0299999999999998</v>
+        <v>0.38</v>
+      </c>
+      <c r="J22" s="19">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>0.38</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="L22" s="21"/>
-      <c r="M22" s="28"/>
+      <c r="M22" s="21"/>
     </row>
     <row r="23" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C23" s="9"/>
       <c r="D23" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>13</v>
@@ -2225,61 +2244,61 @@
         <v>1</v>
       </c>
       <c r="I23" s="18">
-        <v>0.32</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="J23" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.32</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="L23" s="21"/>
-      <c r="M23" s="26"/>
+      <c r="M23" s="28"/>
     </row>
     <row r="24" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C24" s="9"/>
       <c r="D24" s="16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>32</v>
+        <v>112</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="H24" s="17">
         <v>1</v>
       </c>
       <c r="I24" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="J24" s="19">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.3</v>
+        <v>0.32</v>
+      </c>
+      <c r="J24" s="18">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>0.32</v>
       </c>
       <c r="K24" s="22" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="L24" s="21"/>
-      <c r="M24" s="27"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C25" s="9"/>
       <c r="D25" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H25" s="17">
         <v>1</v>
@@ -2292,67 +2311,67 @@
         <v>0.3</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="L25" s="21"/>
-      <c r="M25" s="28"/>
+      <c r="M25" s="27"/>
     </row>
     <row r="26" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C26" s="9"/>
       <c r="D26" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="H26" s="17">
         <v>1</v>
       </c>
       <c r="I26" s="18">
-        <v>0.21</v>
-      </c>
-      <c r="J26" s="18">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.21</v>
+        <v>0.3</v>
+      </c>
+      <c r="J26" s="19">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>0.3</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="L26" s="21"/>
-      <c r="M26" s="27"/>
+      <c r="M26" s="28"/>
     </row>
     <row r="27" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C27" s="9"/>
       <c r="D27" s="16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>181</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="H27" s="17">
         <v>1</v>
       </c>
       <c r="I27" s="18">
-        <v>0.1</v>
+        <v>0.23</v>
       </c>
       <c r="J27" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.1</v>
+        <v>0.23</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="27"/>
@@ -2360,16 +2379,16 @@
     <row r="28" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C28" s="9"/>
       <c r="D28" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>101</v>
+        <v>52</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H28" s="17">
         <v>1</v>
@@ -2382,21 +2401,21 @@
         <v>0.1</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
+      <c r="M28" s="27"/>
     </row>
     <row r="29" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C29" s="9"/>
       <c r="D29" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>102</v>
+        <v>53</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>60</v>
@@ -2405,14 +2424,14 @@
         <v>1</v>
       </c>
       <c r="I29" s="18">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J29" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="L29" s="21"/>
       <c r="M29" s="21"/>
@@ -2420,29 +2439,29 @@
     <row r="30" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C30" s="9"/>
       <c r="D30" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>103</v>
+        <v>47</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>177</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="H30" s="17">
         <v>1</v>
       </c>
       <c r="I30" s="18">
-        <v>0.46</v>
+        <v>0.25</v>
       </c>
       <c r="J30" s="18">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.46</v>
+        <v>0.25</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>82</v>
+        <v>176</v>
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
@@ -2450,29 +2469,29 @@
     <row r="31" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C31" s="9"/>
       <c r="D31" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>104</v>
+        <v>178</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
       <c r="H31" s="17">
         <v>1</v>
       </c>
       <c r="I31" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="J31" s="19">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.1</v>
+        <v>0.37</v>
+      </c>
+      <c r="J31" s="18">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>0.37</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>80</v>
+        <v>179</v>
       </c>
       <c r="L31" s="21"/>
       <c r="M31" s="21"/>
@@ -2480,29 +2499,29 @@
     <row r="32" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C32" s="9"/>
       <c r="D32" s="16" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>106</v>
+        <v>120</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H32" s="17">
         <v>1</v>
       </c>
       <c r="I32" s="18">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J32" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
@@ -2510,29 +2529,29 @@
     <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C33" s="9"/>
       <c r="D33" s="16" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="34" t="s">
-        <v>13</v>
+        <v>118</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="H33" s="17">
         <v>1</v>
       </c>
       <c r="I33" s="18">
-        <v>1.31</v>
-      </c>
-      <c r="J33" s="18">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>1.31</v>
+        <v>0.11</v>
+      </c>
+      <c r="J33" s="19">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>0.11</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="L33" s="21"/>
       <c r="M33" s="21"/>
@@ -2540,13 +2559,13 @@
     <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C34" s="9"/>
       <c r="D34" s="16" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G34" s="34" t="s">
         <v>13</v>
@@ -2555,14 +2574,14 @@
         <v>1</v>
       </c>
       <c r="I34" s="18">
-        <v>0.44</v>
-      </c>
-      <c r="J34" s="19">
-        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.44</v>
+        <v>1.31</v>
+      </c>
+      <c r="J34" s="18">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>1.31</v>
       </c>
       <c r="K34" s="22" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
@@ -2570,29 +2589,29 @@
     <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C35" s="9"/>
       <c r="D35" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="20">
-        <v>3</v>
+      <c r="F35" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="H35" s="17">
         <v>1</v>
       </c>
       <c r="I35" s="18">
-        <v>0.13</v>
+        <v>0.44</v>
       </c>
       <c r="J35" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.13</v>
+        <v>0.44</v>
       </c>
       <c r="K35" s="22" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21"/>
@@ -2600,29 +2619,29 @@
     <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C36" s="9"/>
       <c r="D36" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>33</v>
+        <v>94</v>
+      </c>
+      <c r="G36" s="20">
+        <v>3</v>
       </c>
       <c r="H36" s="17">
         <v>1</v>
       </c>
       <c r="I36" s="18">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="J36" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="K36" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
@@ -2630,29 +2649,29 @@
     <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C37" s="9"/>
       <c r="D37" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>106</v>
+        <v>48</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H37" s="17">
         <v>1</v>
       </c>
       <c r="I37" s="18">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J37" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="K37" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
@@ -2660,29 +2679,29 @@
     <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C38" s="9"/>
       <c r="D38" s="16" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F38" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>13</v>
+        <v>113</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="H38" s="17">
         <v>1</v>
       </c>
       <c r="I38" s="18">
-        <v>0.94</v>
+        <v>0.11</v>
       </c>
       <c r="J38" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.94</v>
+        <v>0.11</v>
       </c>
       <c r="K38" s="22" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="L38" s="21"/>
       <c r="M38" s="21"/>
@@ -2690,29 +2709,29 @@
     <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C39" s="9"/>
       <c r="D39" s="16" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>175</v>
+        <v>147</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="H39" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39" s="18">
-        <v>0.1</v>
+        <v>0.94</v>
       </c>
       <c r="J39" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.2</v>
+        <v>0.94</v>
       </c>
       <c r="K39" s="22" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="L39" s="21"/>
       <c r="M39" s="21"/>
@@ -2720,16 +2739,16 @@
     <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C40" s="9"/>
       <c r="D40" s="16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="20">
-        <v>665</v>
+        <v>167</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="H40" s="17">
         <v>2</v>
@@ -2742,70 +2761,70 @@
         <v>0.2</v>
       </c>
       <c r="K40" s="22" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
     </row>
     <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="10" t="s">
-        <v>167</v>
-      </c>
       <c r="C41" s="9"/>
       <c r="D41" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>38</v>
+        <v>96</v>
+      </c>
+      <c r="G41" s="20">
+        <v>665</v>
       </c>
       <c r="H41" s="17">
         <v>2</v>
       </c>
       <c r="I41" s="18">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J41" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="K41" s="22" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="21"/>
     </row>
     <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="10" t="s">
+        <v>156</v>
+      </c>
       <c r="C42" s="9"/>
       <c r="D42" s="16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H42" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I42" s="18">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="J42" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.30000000000000004</v>
+        <v>0.22</v>
       </c>
       <c r="K42" s="22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
@@ -2813,29 +2832,29 @@
     <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C43" s="9"/>
       <c r="D43" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="H43" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I43" s="18">
         <v>0.1</v>
       </c>
       <c r="J43" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K43" s="22" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
@@ -2843,29 +2862,29 @@
     <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C44" s="9"/>
       <c r="D44" s="16" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H44" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44" s="18">
         <v>0.1</v>
       </c>
       <c r="J44" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K44" s="22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
@@ -2873,43 +2892,60 @@
     <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C45" s="9"/>
       <c r="D45" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>176</v>
+        <v>124</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="H45" s="17">
         <v>1</v>
       </c>
       <c r="I45" s="18">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="J45" s="19">
         <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="K45" s="22" t="s">
-        <v>177</v>
+        <v>77</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="21"/>
     </row>
     <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C46" s="9"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="23"/>
+      <c r="D46" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H46" s="17">
+        <v>1</v>
+      </c>
+      <c r="I46" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="J46" s="19">
+        <f>IFERROR(List3[[#This Row],[QTY]]*List3[[#This Row],[Price]],"")</f>
+        <v>0.8</v>
+      </c>
+      <c r="K46" s="22" t="s">
+        <v>166</v>
+      </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
     </row>
@@ -2919,14 +2955,9 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="J47" s="38">
-        <f>SUM(J4:J45)</f>
-        <v>97.579999999999927</v>
-      </c>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
       <c r="K47" s="23"/>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
@@ -2937,11 +2968,17 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="J48" s="38">
+        <f>SUM(J4:J46)</f>
+        <v>101.56999999999994</v>
+      </c>
       <c r="K48" s="23"/>
       <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
     </row>
     <row r="49" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C49" s="9"/>
@@ -2968,197 +3005,212 @@
       <c r="L50" s="21"/>
     </row>
     <row r="51" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="K51" s="24"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="21"/>
     </row>
     <row r="52" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="K52" s="24"/>
     </row>
+    <row r="53" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K53" s="24"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
-  <conditionalFormatting sqref="H11:J12 C33:K33 C22:J23 C34:J34 C24:E32 G26:J31 C38:J38 C35:E37 G35:J37 C39:E39 G10:J10 C9:J9 C6:E8 G46:I46 K46 E47:K50 G6:J8 G39:J39 G41:J45 C40:C50 C21:E21 C10:E19 G21:J21 G13:J19 F17 C20">
-    <cfRule type="expression" dxfId="28" priority="40">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(C6))</formula>
+  <conditionalFormatting sqref="H12:J13 C34:K34 C23:J24 C35:J35 C25:E33 G27:J32 C39:J39 C36:E38 G36:J38 C40:E40 G11:J11 C10:J10 C7:E9 G47:I47 K47 E48:K51 G7:J9 G40:J40 G42:J46 C41:C51 C22:E22 C11:E20 G22:J22 G14:J20 F18 C21">
+    <cfRule type="expression" dxfId="38" priority="41">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(C7))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
-    <cfRule type="expression" dxfId="27" priority="36">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(L14))</formula>
+  <conditionalFormatting sqref="L15">
+    <cfRule type="expression" dxfId="37" priority="37">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(L15))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G12">
-    <cfRule type="expression" dxfId="26" priority="37">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G11))</formula>
+  <conditionalFormatting sqref="G12:G13">
+    <cfRule type="expression" dxfId="36" priority="38">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G12))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:J4 C5">
-    <cfRule type="expression" dxfId="25" priority="34">
+  <conditionalFormatting sqref="C4:J4 C5:C6">
+    <cfRule type="expression" dxfId="35" priority="35">
       <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(C4))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D46">
-    <cfRule type="expression" dxfId="24" priority="31">
+  <conditionalFormatting sqref="D42:D47">
+    <cfRule type="expression" dxfId="34" priority="32">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D42))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48:D51">
+    <cfRule type="expression" dxfId="33" priority="31">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D48))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F47 E44:E45">
+    <cfRule type="expression" dxfId="32" priority="30">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(E44))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" dxfId="31" priority="29">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(E42))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="expression" dxfId="30" priority="28">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(E43))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K42">
+    <cfRule type="expression" dxfId="29" priority="26">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K42))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="expression" dxfId="28" priority="25">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K31))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="expression" dxfId="27" priority="23">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K29))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40">
+    <cfRule type="expression" dxfId="26" priority="22">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K40))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
+    <cfRule type="expression" dxfId="25" priority="21">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K36))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K44">
+    <cfRule type="expression" dxfId="24" priority="20">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K44))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46">
+    <cfRule type="expression" dxfId="23" priority="19">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K46))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="expression" dxfId="22" priority="17">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K17))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47">
+    <cfRule type="expression" dxfId="21" priority="16">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(J47))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33:J33">
+    <cfRule type="expression" dxfId="20" priority="14">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G33))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" dxfId="19" priority="13">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F8))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="18" priority="10">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:E6 G5:J6">
+    <cfRule type="expression" dxfId="17" priority="12">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="16" priority="8">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:J25">
+    <cfRule type="expression" dxfId="15" priority="7">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G25))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26:J26">
+    <cfRule type="expression" dxfId="14" priority="6">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G26))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="expression" dxfId="13" priority="5">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:E41 G41:J41">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D41))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47:D50">
-    <cfRule type="expression" dxfId="23" priority="30">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D47))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:F46 E43:E44">
-    <cfRule type="expression" dxfId="22" priority="29">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(E43))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="21" priority="28">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(E41))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="20" priority="27">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(E42))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K41">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K41))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
-    <cfRule type="expression" dxfId="18" priority="24">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K30))</formula>
+  <conditionalFormatting sqref="D21:E21 G21:J21">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D21))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
-    <cfRule type="expression" dxfId="17" priority="22">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K28))</formula>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F6))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K39">
-    <cfRule type="expression" dxfId="16" priority="21">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K39))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
-    <cfRule type="expression" dxfId="15" priority="20">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K35))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="14" priority="19">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K43))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="expression" dxfId="13" priority="18">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K45))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K16))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(J46))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:J32">
-    <cfRule type="expression" dxfId="10" priority="13">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G32))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="9" priority="12">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F7))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:E5 G5:J5">
-    <cfRule type="expression" dxfId="7" priority="11">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(F15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G24:J24">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G24))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25:J25">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(G25))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40:E40 G40:J40">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D40))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K40">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(K40))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20:E20 G20:J20">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISODD(ROW(TableAnchor))&lt;&gt;ISODD(ROW(D20))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations xWindow="930" yWindow="374" count="11">
+  <dataValidations xWindow="883" yWindow="440" count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter grocery details in table below. Category totals are automatically updated in column M" sqref="B2:L2" xr:uid="{C36C3168-609D-4C36-87F2-5C6B314746B2}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Comment in this column under this heading" sqref="K3" xr:uid="{AB6EB83F-5CF9-4686-8E06-F4AF7445A6F3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Category in this column under this heading" sqref="F3:F4 G3:G5" xr:uid="{C2FB87D2-E049-4B57-82ED-57CB1B262B0D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Category in this column under this heading" sqref="F3:F4 G3:G6" xr:uid="{C2FB87D2-E049-4B57-82ED-57CB1B262B0D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Grocery List in this worksheet. Enter details in List table. Totals are automatically calculated" sqref="A1" xr:uid="{6973CA39-0F95-4978-AD3F-A91AA8A24FC5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total is automatically calculated in this column under this heading" sqref="J3:J5" xr:uid="{ACE1844F-CD21-40CE-8F29-EF968E5CA803}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit Price in this column under this heading" sqref="I3:I5" xr:uid="{B09114CB-23D3-4599-B062-90EEE9700C36}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit in this column under this heading" sqref="G3:G5" xr:uid="{6031E46B-B175-4CFB-9C40-CC7166B7A0E4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in this column under this heading" sqref="H3:H5" xr:uid="{08DD1F1F-ABA9-4B55-A622-0A0E724CB08F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Store type in this column under this heading" sqref="E3:E5" xr:uid="{3D501318-E80D-4C59-A8E7-1E82B37D74B1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Item in this column under this heading" sqref="D3:D5" xr:uid="{9F00BFCE-1EF7-470C-A2C3-8EA1042E9CFC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0 in this column under this heading to mark item as bought. Use heading filters to find specific entries" sqref="C3:C5" xr:uid="{5B52AA20-747F-43BF-B8BD-4FB9BAB672C1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total is automatically calculated in this column under this heading" sqref="J3:J6" xr:uid="{ACE1844F-CD21-40CE-8F29-EF968E5CA803}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit Price in this column under this heading" sqref="I3:I6" xr:uid="{B09114CB-23D3-4599-B062-90EEE9700C36}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit in this column under this heading" sqref="G3:G6" xr:uid="{6031E46B-B175-4CFB-9C40-CC7166B7A0E4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Quantity in this column under this heading" sqref="H3:H6" xr:uid="{08DD1F1F-ABA9-4B55-A622-0A0E724CB08F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Store type in this column under this heading" sqref="E3:E6" xr:uid="{3D501318-E80D-4C59-A8E7-1E82B37D74B1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Item in this column under this heading" sqref="D3:D6" xr:uid="{9F00BFCE-1EF7-470C-A2C3-8EA1042E9CFC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0 in this column under this heading to mark item as bought. Use heading filters to find specific entries" sqref="C3:C6" xr:uid="{5B52AA20-747F-43BF-B8BD-4FB9BAB672C1}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{44F63769-758D-4CF4-83A6-A90FACC43A51}"/>
-    <hyperlink ref="K10" r:id="rId2" xr:uid="{CAA4BF09-AEC4-4C2C-8CA4-15B7C61E9C07}"/>
-    <hyperlink ref="K21" r:id="rId3" xr:uid="{8AF97949-1A13-4DB4-9660-BCD527C707B3}"/>
-    <hyperlink ref="K22" r:id="rId4" xr:uid="{3A54EFBB-3D5A-42C9-A27F-F329C3333723}"/>
-    <hyperlink ref="K14" r:id="rId5" xr:uid="{9968FDC6-1466-44E5-B497-CC59831D2A05}"/>
+    <hyperlink ref="K11" r:id="rId2" xr:uid="{CAA4BF09-AEC4-4C2C-8CA4-15B7C61E9C07}"/>
+    <hyperlink ref="K22" r:id="rId3" xr:uid="{8AF97949-1A13-4DB4-9660-BCD527C707B3}"/>
+    <hyperlink ref="K23" r:id="rId4" xr:uid="{3A54EFBB-3D5A-42C9-A27F-F329C3333723}"/>
+    <hyperlink ref="K15" r:id="rId5" xr:uid="{9968FDC6-1466-44E5-B497-CC59831D2A05}"/>
     <hyperlink ref="K4" r:id="rId6" location="1" xr:uid="{6E6F4268-3326-4B19-B83F-E58D19ED4FDD}"/>
-    <hyperlink ref="K9" r:id="rId7" xr:uid="{E5247556-AD3C-4E2E-92B4-7854AA584826}"/>
+    <hyperlink ref="K10" r:id="rId7" xr:uid="{E5247556-AD3C-4E2E-92B4-7854AA584826}"/>
+    <hyperlink ref="K25" r:id="rId8" xr:uid="{D9AE72CB-7E04-47F0-892A-3CC3DB8FB579}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="55" fitToHeight="0" orientation="portrait" r:id="rId8"/>
+  <pageSetup scale="55" fitToHeight="0" orientation="portrait" r:id="rId9"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="J47" calculatedColumn="1"/>
-  </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="71" id="{E4215F6E-1F3A-439C-81DA-C4F538E7C55C}">
+          <x14:cfRule type="iconSet" priority="72" id="{E4215F6E-1F3A-439C-81DA-C4F538E7C55C}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3174,10 +3226,10 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C4:C5</xm:sqref>
+          <xm:sqref>C4:C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="72" id="{AB3A6594-1896-46F4-975E-45A22D8D27CD}">
+          <x14:cfRule type="iconSet" priority="73" id="{AB3A6594-1896-46F4-975E-45A22D8D27CD}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3193,7 +3245,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C6:C50</xm:sqref>
+          <xm:sqref>C7:C51</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>